<commit_message>
allcourse and course data
</commit_message>
<xml_diff>
--- a/dev_includes/Test_Data/course.xlsx
+++ b/dev_includes/Test_Data/course.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihir\OneDrive\Desktop\Database_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1A54DC-4754-4DAF-9E0E-9CAF46E67216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8EABA-9F89-46A1-A037-28E9AA27AAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{67CA327F-CE57-494E-AB70-1709CD8B124C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{67CA327F-CE57-494E-AB70-1709CD8B124C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,46 +28,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>EC6010</t>
-  </si>
-  <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>COM002</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>Software Engineering</t>
   </si>
   <si>
-    <t>COM003</t>
-  </si>
-  <si>
     <t>EC6060</t>
   </si>
   <si>
     <t>EC9630</t>
   </si>
   <si>
-    <t xml:space="preserve">machine learning </t>
-  </si>
-  <si>
-    <t>Technical</t>
+    <t>Course_code</t>
+  </si>
+  <si>
+    <t>Course_Name</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Core_Technical</t>
+  </si>
+  <si>
+    <t>Coordinator_ID</t>
+  </si>
+  <si>
+    <t>Offered_Semester</t>
+  </si>
+  <si>
+    <t>Offered_Department_ID</t>
+  </si>
+  <si>
+    <t>Academic_Year_Current</t>
+  </si>
+  <si>
+    <t>Registratipon_Open_Date</t>
+  </si>
+  <si>
+    <t>    Registration_Close_Date</t>
+  </si>
+  <si>
+    <t>Semester_Start_Date</t>
+  </si>
+  <si>
+    <t>Semester_Close_Date</t>
+  </si>
+  <si>
+    <t>Open_Close</t>
+  </si>
+  <si>
+    <t>EC6020</t>
+  </si>
+  <si>
+    <t>Embedded Systems Design</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>EC6110</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>EC6070</t>
+  </si>
+  <si>
+    <t>Computer Engineering Research Project I</t>
+  </si>
+  <si>
+    <t>EC6090</t>
+  </si>
+  <si>
+    <t>Robotics and Automation</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>COM001</t>
+  </si>
+  <si>
+    <t>20/07/2023</t>
+  </si>
+  <si>
+    <t>30/07/2023</t>
+  </si>
+  <si>
+    <t>30/07/2024</t>
+  </si>
+  <si>
+    <t>30/07/2025</t>
+  </si>
+  <si>
+    <t>30/07/2026</t>
+  </si>
+  <si>
+    <t>30/07/2027</t>
+  </si>
+  <si>
+    <t>30/07/2028</t>
+  </si>
+  <si>
+    <t>18/07/2023</t>
+  </si>
+  <si>
+    <t>30/09/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,9 +189,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,6 +214,120 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>EC5010</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>Digital Signal Processing</v>
+          </cell>
+          <cell r="C26">
+            <v>3</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>core</v>
+          </cell>
+          <cell r="E26">
+            <v>5</v>
+          </cell>
+          <cell r="F26" t="str">
+            <v>COM</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>EC5020</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>Analogue and Communication</v>
+          </cell>
+          <cell r="C27">
+            <v>3</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>core</v>
+          </cell>
+          <cell r="E27">
+            <v>5</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>COM</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>EC5030</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Control Systems</v>
+          </cell>
+          <cell r="C28">
+            <v>3</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>core</v>
+          </cell>
+          <cell r="E28">
+            <v>5</v>
+          </cell>
+          <cell r="F28" t="str">
+            <v>COM</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>EC5070</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>Database Systems</v>
+          </cell>
+          <cell r="C29">
+            <v>3</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>core</v>
+          </cell>
+          <cell r="E29">
+            <v>5</v>
+          </cell>
+          <cell r="F29" t="str">
+            <v>COM</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>EC5080</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>Software construction</v>
+          </cell>
+          <cell r="C30">
+            <v>3</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>core</v>
+          </cell>
+          <cell r="E30">
+            <v>5</v>
+          </cell>
+          <cell r="F30" t="str">
+            <v>COM</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA774EF-492A-4CAC-8150-001CAF7E4E27}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
@@ -415,122 +635,545 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" customWidth="1"/>
+    <col min="10" max="11" width="23.109375" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>6</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>2023</v>
-      </c>
-      <c r="I1" s="1">
-        <v>45036</v>
-      </c>
-      <c r="J1" s="1">
-        <v>45170</v>
-      </c>
-      <c r="K1">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>19</v>
       </c>
       <c r="H2">
         <v>2023</v>
       </c>
-      <c r="I2" s="1">
-        <v>45036</v>
-      </c>
-      <c r="J2" s="1">
-        <v>45170</v>
-      </c>
-      <c r="K2">
+      <c r="I2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>2023</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>2023</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>2023</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>2023</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>2023</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>[1]Sheet1!A26</f>
+        <v>EC5010</v>
+      </c>
+      <c r="B8" t="str">
+        <f>[1]Sheet1!B26</f>
+        <v>Digital Signal Processing</v>
+      </c>
+      <c r="C8">
+        <f>[1]Sheet1!C26</f>
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
+      <c r="D8" t="str">
+        <f>[1]Sheet1!D26</f>
+        <v>core</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <f>[1]Sheet1!E26</f>
+        <v>5</v>
+      </c>
+      <c r="G8" t="str">
+        <f>[1]Sheet1!F26</f>
+        <v>COM</v>
+      </c>
+      <c r="H8">
+        <v>2023</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:J3" si="0">H2</f>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>[1]Sheet1!A27</f>
+        <v>EC5020</v>
+      </c>
+      <c r="B9" t="str">
+        <f>[1]Sheet1!B27</f>
+        <v>Analogue and Communication</v>
+      </c>
+      <c r="C9">
+        <f>[1]Sheet1!C27</f>
+        <v>3</v>
+      </c>
+      <c r="D9" t="str">
+        <f>[1]Sheet1!D27</f>
+        <v>core</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9">
+        <f>[1]Sheet1!E27</f>
+        <v>5</v>
+      </c>
+      <c r="G9" t="str">
+        <f>[1]Sheet1!F27</f>
+        <v>COM</v>
+      </c>
+      <c r="H9">
         <v>2023</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:J3" si="1">I2</f>
-        <v>45036</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" si="1"/>
-        <v>45170</v>
-      </c>
-      <c r="K3">
+      <c r="I9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>[1]Sheet1!A28</f>
+        <v>EC5030</v>
+      </c>
+      <c r="B10" t="str">
+        <f>[1]Sheet1!B28</f>
+        <v>Control Systems</v>
+      </c>
+      <c r="C10">
+        <f>[1]Sheet1!C28</f>
+        <v>3</v>
+      </c>
+      <c r="D10" t="str">
+        <f>[1]Sheet1!D28</f>
+        <v>core</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <f>[1]Sheet1!E28</f>
+        <v>5</v>
+      </c>
+      <c r="G10" t="str">
+        <f>[1]Sheet1!F28</f>
+        <v>COM</v>
+      </c>
+      <c r="H10">
+        <v>2023</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>[1]Sheet1!A29</f>
+        <v>EC5070</v>
+      </c>
+      <c r="B11" t="str">
+        <f>[1]Sheet1!B29</f>
+        <v>Database Systems</v>
+      </c>
+      <c r="C11">
+        <f>[1]Sheet1!C29</f>
+        <v>3</v>
+      </c>
+      <c r="D11" t="str">
+        <f>[1]Sheet1!D29</f>
+        <v>core</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <f>[1]Sheet1!E29</f>
+        <v>5</v>
+      </c>
+      <c r="G11" t="str">
+        <f>[1]Sheet1!F29</f>
+        <v>COM</v>
+      </c>
+      <c r="H11">
+        <v>2023</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>[1]Sheet1!A30</f>
+        <v>EC5080</v>
+      </c>
+      <c r="B12" t="str">
+        <f>[1]Sheet1!B30</f>
+        <v>Software construction</v>
+      </c>
+      <c r="C12">
+        <f>[1]Sheet1!C30</f>
+        <v>3</v>
+      </c>
+      <c r="D12" t="str">
+        <f>[1]Sheet1!D30</f>
+        <v>core</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <f>[1]Sheet1!E30</f>
+        <v>5</v>
+      </c>
+      <c r="G12" t="str">
+        <f>[1]Sheet1!F30</f>
+        <v>COM</v>
+      </c>
+      <c r="H12">
+        <v>2023</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>